<commit_message>
added environment & reworked optimisation
</commit_message>
<xml_diff>
--- a/config/optimal-schedule.xlsx
+++ b/config/optimal-schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxime.ferard\Documents\Github - personal\osiris\main\parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxim\Documents\Github\osiris\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B411E5-C000-4FF8-8AAA-1371C5319253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E407450-7A41-4273-9266-022943253AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{6DB6AD8B-4684-4BE4-AD3F-5DFF7E0CF8D2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6DB6AD8B-4684-4BE4-AD3F-5DFF7E0CF8D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="8">
   <si>
     <t>sleep</t>
   </si>
@@ -58,6 +58,9 @@
   <si>
     <t>working-day</t>
   </si>
+  <si>
+    <t>cleanup</t>
+  </si>
 </sst>
 </file>
 
@@ -72,7 +75,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -109,6 +112,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -122,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -131,6 +140,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -963,8 +973,8 @@
       <c r="A36" s="2">
         <v>0.36458333333333343</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>1</v>
+      <c r="B36" s="6" t="s">
+        <v>3</v>
       </c>
       <c r="D36" s="2">
         <v>0.36458333333333343</v>
@@ -1123,8 +1133,8 @@
       <c r="D47" s="2">
         <v>0.47916666666666696</v>
       </c>
-      <c r="E47" s="4" t="s">
-        <v>1</v>
+      <c r="E47" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1137,8 +1147,8 @@
       <c r="D48" s="2">
         <v>0.48958333333333365</v>
       </c>
-      <c r="E48" s="4" t="s">
-        <v>1</v>
+      <c r="E48" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1151,8 +1161,8 @@
       <c r="D49" s="2">
         <v>0.50000000000000033</v>
       </c>
-      <c r="E49" s="4" t="s">
-        <v>1</v>
+      <c r="E49" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1165,8 +1175,8 @@
       <c r="D50" s="2">
         <v>0.51041666666666696</v>
       </c>
-      <c r="E50" s="4" t="s">
-        <v>1</v>
+      <c r="E50" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1179,8 +1189,8 @@
       <c r="D51" s="2">
         <v>0.52083333333333359</v>
       </c>
-      <c r="E51" s="4" t="s">
-        <v>1</v>
+      <c r="E51" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1193,8 +1203,8 @@
       <c r="D52" s="2">
         <v>0.53125000000000022</v>
       </c>
-      <c r="E52" s="4" t="s">
-        <v>1</v>
+      <c r="E52" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1207,8 +1217,8 @@
       <c r="D53" s="2">
         <v>0.54166666666666685</v>
       </c>
-      <c r="E53" s="4" t="s">
-        <v>1</v>
+      <c r="E53" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1243,28 +1253,28 @@
       <c r="A56" s="2">
         <v>0.57291666666666674</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>1</v>
+      <c r="B56" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="D56" s="2">
         <v>0.57291666666666674</v>
       </c>
-      <c r="E56" s="4" t="s">
-        <v>1</v>
+      <c r="E56" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="B57" s="4" t="s">
-        <v>1</v>
+      <c r="B57" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="D57" s="2">
         <v>0.58333333333333337</v>
       </c>
-      <c r="E57" s="4" t="s">
-        <v>1</v>
+      <c r="E57" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1277,8 +1287,8 @@
       <c r="D58" s="2">
         <v>0.59375</v>
       </c>
-      <c r="E58" s="4" t="s">
-        <v>1</v>
+      <c r="E58" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1291,8 +1301,8 @@
       <c r="D59" s="2">
         <v>0.60416666666666663</v>
       </c>
-      <c r="E59" s="4" t="s">
-        <v>1</v>
+      <c r="E59" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1305,8 +1315,8 @@
       <c r="D60" s="2">
         <v>0.61458333333333326</v>
       </c>
-      <c r="E60" s="4" t="s">
-        <v>1</v>
+      <c r="E60" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1319,8 +1329,8 @@
       <c r="D61" s="2">
         <v>0.62499999999999989</v>
       </c>
-      <c r="E61" s="4" t="s">
-        <v>1</v>
+      <c r="E61" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1333,8 +1343,8 @@
       <c r="D62" s="2">
         <v>0.63541666666666652</v>
       </c>
-      <c r="E62" s="4" t="s">
-        <v>1</v>
+      <c r="E62" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1459,8 +1469,8 @@
       <c r="D71" s="2">
         <v>0.72916666666666619</v>
       </c>
-      <c r="E71" s="7" t="s">
-        <v>4</v>
+      <c r="E71" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -1473,8 +1483,8 @@
       <c r="D72" s="2">
         <v>0.73958333333333282</v>
       </c>
-      <c r="E72" s="7" t="s">
-        <v>4</v>
+      <c r="E72" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -1487,8 +1497,8 @@
       <c r="D73" s="2">
         <v>0.74999999999999944</v>
       </c>
-      <c r="E73" s="4" t="s">
-        <v>1</v>
+      <c r="E73" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -1501,8 +1511,8 @@
       <c r="D74" s="2">
         <v>0.76041666666666607</v>
       </c>
-      <c r="E74" s="4" t="s">
-        <v>1</v>
+      <c r="E74" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -1515,8 +1525,8 @@
       <c r="D75" s="2">
         <v>0.7708333333333327</v>
       </c>
-      <c r="E75" s="4" t="s">
-        <v>1</v>
+      <c r="E75" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -1529,8 +1539,8 @@
       <c r="D76" s="2">
         <v>0.78124999999999933</v>
       </c>
-      <c r="E76" s="4" t="s">
-        <v>1</v>
+      <c r="E76" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -1543,8 +1553,8 @@
       <c r="D77" s="2">
         <v>0.79166666666666596</v>
       </c>
-      <c r="E77" s="4" t="s">
-        <v>1</v>
+      <c r="E77" s="8" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -1607,8 +1617,8 @@
       <c r="A82" s="2">
         <v>0.84374999999999911</v>
       </c>
-      <c r="B82" s="7" t="s">
-        <v>4</v>
+      <c r="B82" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="D82" s="2">
         <v>0.84374999999999911</v>
@@ -1621,8 +1631,8 @@
       <c r="A83" s="2">
         <v>0.85416666666666574</v>
       </c>
-      <c r="B83" s="7" t="s">
-        <v>4</v>
+      <c r="B83" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="D83" s="2">
         <v>0.85416666666666574</v>
@@ -1719,42 +1729,42 @@
       <c r="A90" s="2">
         <v>0.92708333333333215</v>
       </c>
-      <c r="B90" s="4" t="s">
-        <v>1</v>
+      <c r="B90" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="D90" s="2">
         <v>0.92708333333333215</v>
       </c>
-      <c r="E90" s="4" t="s">
-        <v>1</v>
+      <c r="E90" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>0.93749999999999878</v>
       </c>
-      <c r="B91" s="4" t="s">
-        <v>1</v>
+      <c r="B91" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="D91" s="2">
         <v>0.93749999999999878</v>
       </c>
-      <c r="E91" s="4" t="s">
-        <v>1</v>
+      <c r="E91" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>0.94791666666666541</v>
       </c>
-      <c r="B92" s="4" t="s">
-        <v>1</v>
+      <c r="B92" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="D92" s="2">
         <v>0.94791666666666541</v>
       </c>
-      <c r="E92" s="4" t="s">
-        <v>1</v>
+      <c r="E92" s="7" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>